<commit_message>
Calculate annual avg cylinder consumption for a HH
</commit_message>
<xml_diff>
--- a/Across survey analysis/LPG and firewood statistics/TM - LPG analysis 4Apr25.xlsx
+++ b/Across survey analysis/LPG and firewood statistics/TM - LPG analysis 4Apr25.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20416"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\KG TM - Joint projects\HCES\Across survey analysis\LPG and firewood statistics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\.shortcut-targets-by-id\1e8tUHTxt5bH6F4EoPeKOxMyma7YF_D0n\KG TM - Joint projects\HCES\Across survey analysis\LPG and firewood statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF51217-B100-4A5E-9612-49BBE0B7C753}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15530" windowHeight="6930" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15530" windowHeight="6930" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Primary cooking source" sheetId="1" r:id="rId1"/>
     <sheet name="LPG subsidy" sheetId="2" r:id="rId2"/>
     <sheet name="Subsidized cylinder count" sheetId="3" r:id="rId3"/>
-    <sheet name="Average consumption" sheetId="4" r:id="rId4"/>
-    <sheet name="PPAC vs HCES lpg consumption" sheetId="5" r:id="rId5"/>
+    <sheet name="Average consumption - PC 30 day" sheetId="4" r:id="rId4"/>
+    <sheet name="Average cylinders - HH 1 yr" sheetId="6" r:id="rId5"/>
+    <sheet name="PPAC vs HCES lpg consumption" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="131">
   <si>
     <t>sample_size</t>
   </si>
@@ -424,11 +426,17 @@
   <si>
     <t>Consumption (OMC + PMS) as per PPAC</t>
   </si>
+  <si>
+    <t># of cylinders</t>
+  </si>
+  <si>
+    <t>All India</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="0.0"/>
@@ -530,7 +538,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -833,6 +841,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -840,7 +861,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -991,6 +1012,38 @@
     <xf numFmtId="167" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1063,15 +1116,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1354,11 +1398,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB65"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="80" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView zoomScale="80" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1379,36 +1423,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="96" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="81" t="s">
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="97"/>
+      <c r="L1" s="97"/>
+      <c r="M1" s="98"/>
+      <c r="N1" s="99" t="s">
         <v>50</v>
       </c>
-      <c r="O1" s="82"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="82"/>
-      <c r="R1" s="82"/>
-      <c r="S1" s="82"/>
-      <c r="T1" s="82"/>
-      <c r="U1" s="82"/>
-      <c r="V1" s="82"/>
-      <c r="W1" s="82"/>
-      <c r="X1" s="82"/>
-      <c r="Y1" s="82"/>
-      <c r="Z1" s="82"/>
+      <c r="O1" s="100"/>
+      <c r="P1" s="100"/>
+      <c r="Q1" s="100"/>
+      <c r="R1" s="100"/>
+      <c r="S1" s="100"/>
+      <c r="T1" s="100"/>
+      <c r="U1" s="100"/>
+      <c r="V1" s="100"/>
+      <c r="W1" s="100"/>
+      <c r="X1" s="100"/>
+      <c r="Y1" s="100"/>
+      <c r="Z1" s="100"/>
       <c r="AA1" s="50"/>
       <c r="AB1" s="51"/>
     </row>
@@ -3780,7 +3824,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AD25"/>
   <sheetViews>
     <sheetView zoomScale="75" workbookViewId="0">
@@ -3805,38 +3849,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="101" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="81" t="s">
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="102"/>
+      <c r="E1" s="102"/>
+      <c r="F1" s="102"/>
+      <c r="G1" s="102"/>
+      <c r="H1" s="102"/>
+      <c r="I1" s="102"/>
+      <c r="J1" s="102"/>
+      <c r="K1" s="102"/>
+      <c r="L1" s="102"/>
+      <c r="M1" s="102"/>
+      <c r="N1" s="102"/>
+      <c r="O1" s="99" t="s">
         <v>50</v>
       </c>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="82"/>
-      <c r="R1" s="82"/>
-      <c r="S1" s="82"/>
-      <c r="T1" s="82"/>
-      <c r="U1" s="82"/>
-      <c r="V1" s="82"/>
-      <c r="W1" s="82"/>
-      <c r="X1" s="82"/>
-      <c r="Y1" s="82"/>
-      <c r="Z1" s="82"/>
-      <c r="AA1" s="82"/>
-      <c r="AB1" s="82"/>
+      <c r="P1" s="100"/>
+      <c r="Q1" s="100"/>
+      <c r="R1" s="100"/>
+      <c r="S1" s="100"/>
+      <c r="T1" s="100"/>
+      <c r="U1" s="100"/>
+      <c r="V1" s="100"/>
+      <c r="W1" s="100"/>
+      <c r="X1" s="100"/>
+      <c r="Y1" s="100"/>
+      <c r="Z1" s="100"/>
+      <c r="AA1" s="100"/>
+      <c r="AB1" s="100"/>
       <c r="AC1" s="50"/>
       <c r="AD1" s="51"/>
     </row>
@@ -4452,11 +4496,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AB31"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="95" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21:K23"/>
+    <sheetView topLeftCell="A15" zoomScale="95" workbookViewId="0">
+      <selection activeCell="Q31" sqref="Q31:Z31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4474,38 +4518,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="29" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="101" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="81" t="s">
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="102"/>
+      <c r="E1" s="102"/>
+      <c r="F1" s="102"/>
+      <c r="G1" s="102"/>
+      <c r="H1" s="102"/>
+      <c r="I1" s="102"/>
+      <c r="J1" s="102"/>
+      <c r="K1" s="102"/>
+      <c r="L1" s="102"/>
+      <c r="M1" s="105"/>
+      <c r="N1" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="O1" s="82"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="82"/>
-      <c r="R1" s="82"/>
-      <c r="S1" s="82"/>
-      <c r="T1" s="82"/>
-      <c r="U1" s="82"/>
-      <c r="V1" s="82"/>
-      <c r="W1" s="82"/>
-      <c r="X1" s="82"/>
-      <c r="Y1" s="82"/>
-      <c r="Z1" s="82"/>
-      <c r="AA1" s="82"/>
-      <c r="AB1" s="85"/>
+      <c r="O1" s="100"/>
+      <c r="P1" s="100"/>
+      <c r="Q1" s="100"/>
+      <c r="R1" s="100"/>
+      <c r="S1" s="100"/>
+      <c r="T1" s="100"/>
+      <c r="U1" s="100"/>
+      <c r="V1" s="100"/>
+      <c r="W1" s="100"/>
+      <c r="X1" s="100"/>
+      <c r="Y1" s="100"/>
+      <c r="Z1" s="100"/>
+      <c r="AA1" s="100"/>
+      <c r="AB1" s="103"/>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
@@ -4732,39 +4776,39 @@
       <c r="Z18" s="41"/>
     </row>
     <row r="19" spans="1:26" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="88" t="s">
+      <c r="A19" s="106" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="86" t="s">
+      <c r="B19" s="104" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="86"/>
-      <c r="D19" s="86"/>
-      <c r="E19" s="86"/>
-      <c r="F19" s="86"/>
-      <c r="G19" s="86"/>
-      <c r="H19" s="86"/>
-      <c r="I19" s="86"/>
-      <c r="J19" s="86"/>
-      <c r="K19" s="86"/>
-      <c r="P19" s="91" t="s">
+      <c r="C19" s="104"/>
+      <c r="D19" s="104"/>
+      <c r="E19" s="104"/>
+      <c r="F19" s="104"/>
+      <c r="G19" s="104"/>
+      <c r="H19" s="104"/>
+      <c r="I19" s="104"/>
+      <c r="J19" s="104"/>
+      <c r="K19" s="104"/>
+      <c r="P19" s="109" t="s">
         <v>29</v>
       </c>
-      <c r="Q19" s="90" t="s">
+      <c r="Q19" s="108" t="s">
         <v>48</v>
       </c>
-      <c r="R19" s="90"/>
-      <c r="S19" s="90"/>
-      <c r="T19" s="90"/>
-      <c r="U19" s="90"/>
-      <c r="V19" s="90"/>
-      <c r="W19" s="90"/>
-      <c r="X19" s="90"/>
-      <c r="Y19" s="90"/>
-      <c r="Z19" s="90"/>
+      <c r="R19" s="108"/>
+      <c r="S19" s="108"/>
+      <c r="T19" s="108"/>
+      <c r="U19" s="108"/>
+      <c r="V19" s="108"/>
+      <c r="W19" s="108"/>
+      <c r="X19" s="108"/>
+      <c r="Y19" s="108"/>
+      <c r="Z19" s="108"/>
     </row>
     <row r="20" spans="1:26" ht="13" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="89"/>
+      <c r="A20" s="107"/>
       <c r="B20" s="2">
         <v>1</v>
       </c>
@@ -4795,7 +4839,7 @@
       <c r="K20" s="2">
         <v>10</v>
       </c>
-      <c r="P20" s="91"/>
+      <c r="P20" s="109"/>
       <c r="Q20" s="43">
         <v>1</v>
       </c>
@@ -5050,39 +5094,39 @@
       <c r="Z26" s="41"/>
     </row>
     <row r="27" spans="1:26" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="88" t="s">
+      <c r="A27" s="106" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="86" t="s">
+      <c r="B27" s="104" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="86"/>
-      <c r="D27" s="86"/>
-      <c r="E27" s="86"/>
-      <c r="F27" s="86"/>
-      <c r="G27" s="86"/>
-      <c r="H27" s="86"/>
-      <c r="I27" s="86"/>
-      <c r="J27" s="86"/>
-      <c r="K27" s="86"/>
-      <c r="P27" s="91" t="s">
+      <c r="C27" s="104"/>
+      <c r="D27" s="104"/>
+      <c r="E27" s="104"/>
+      <c r="F27" s="104"/>
+      <c r="G27" s="104"/>
+      <c r="H27" s="104"/>
+      <c r="I27" s="104"/>
+      <c r="J27" s="104"/>
+      <c r="K27" s="104"/>
+      <c r="P27" s="109" t="s">
         <v>29</v>
       </c>
-      <c r="Q27" s="90" t="s">
+      <c r="Q27" s="108" t="s">
         <v>48</v>
       </c>
-      <c r="R27" s="90"/>
-      <c r="S27" s="90"/>
-      <c r="T27" s="90"/>
-      <c r="U27" s="90"/>
-      <c r="V27" s="90"/>
-      <c r="W27" s="90"/>
-      <c r="X27" s="90"/>
-      <c r="Y27" s="90"/>
-      <c r="Z27" s="90"/>
+      <c r="R27" s="108"/>
+      <c r="S27" s="108"/>
+      <c r="T27" s="108"/>
+      <c r="U27" s="108"/>
+      <c r="V27" s="108"/>
+      <c r="W27" s="108"/>
+      <c r="X27" s="108"/>
+      <c r="Y27" s="108"/>
+      <c r="Z27" s="108"/>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A28" s="89"/>
+      <c r="A28" s="107"/>
       <c r="B28" s="2">
         <v>1</v>
       </c>
@@ -5113,7 +5157,7 @@
       <c r="K28" s="2">
         <v>10</v>
       </c>
-      <c r="P28" s="91"/>
+      <c r="P28" s="109"/>
       <c r="Q28" s="43">
         <v>1</v>
       </c>
@@ -5367,11 +5411,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AD187"/>
   <sheetViews>
-    <sheetView zoomScale="74" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView topLeftCell="A49" zoomScale="51" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5393,40 +5437,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="29" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="101" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="87"/>
-      <c r="O1" s="81" t="s">
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="102"/>
+      <c r="E1" s="102"/>
+      <c r="F1" s="102"/>
+      <c r="G1" s="102"/>
+      <c r="H1" s="102"/>
+      <c r="I1" s="102"/>
+      <c r="J1" s="102"/>
+      <c r="K1" s="102"/>
+      <c r="L1" s="102"/>
+      <c r="M1" s="102"/>
+      <c r="N1" s="105"/>
+      <c r="O1" s="99" t="s">
         <v>50</v>
       </c>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="82"/>
-      <c r="R1" s="82"/>
-      <c r="S1" s="82"/>
-      <c r="T1" s="82"/>
-      <c r="U1" s="82"/>
-      <c r="V1" s="82"/>
-      <c r="W1" s="82"/>
-      <c r="X1" s="82"/>
-      <c r="Y1" s="82"/>
-      <c r="Z1" s="82"/>
-      <c r="AA1" s="82"/>
-      <c r="AB1" s="82"/>
-      <c r="AC1" s="82"/>
-      <c r="AD1" s="85"/>
+      <c r="P1" s="100"/>
+      <c r="Q1" s="100"/>
+      <c r="R1" s="100"/>
+      <c r="S1" s="100"/>
+      <c r="T1" s="100"/>
+      <c r="U1" s="100"/>
+      <c r="V1" s="100"/>
+      <c r="W1" s="100"/>
+      <c r="X1" s="100"/>
+      <c r="Y1" s="100"/>
+      <c r="Z1" s="100"/>
+      <c r="AA1" s="100"/>
+      <c r="AB1" s="100"/>
+      <c r="AC1" s="100"/>
+      <c r="AD1" s="103"/>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
@@ -5508,7 +5552,7 @@
       </c>
       <c r="C8" s="34">
         <f>C7/(C6*$G$9*$H$9)</f>
-        <v>2.6680937716990845</v>
+        <v>2.5569231978782887</v>
       </c>
       <c r="F8" s="70"/>
       <c r="G8" s="72" t="s">
@@ -5525,7 +5569,7 @@
       </c>
       <c r="S8" s="56">
         <f>S7/(S6*$G$9*$H$9)</f>
-        <v>2.2197982820475732</v>
+        <v>2.1273066869622577</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.35">
@@ -5542,7 +5586,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="70">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H9" s="70">
         <v>0.65</v>
@@ -5674,10 +5718,10 @@
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A17" s="15"/>
-      <c r="C17" s="92" t="s">
+      <c r="C17" s="110" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="92"/>
+      <c r="D17" s="110"/>
       <c r="Q17" s="41"/>
       <c r="R17" s="41"/>
       <c r="S17" s="41" t="s">
@@ -5792,11 +5836,11 @@
       </c>
       <c r="C21" s="34">
         <f>C20/(C19*$G$9*$H$9)</f>
-        <v>2.6857439296251671</v>
+        <v>2.5738379325574523</v>
       </c>
       <c r="D21" s="34">
         <f>D20/(D19*$G$9*$H$9)</f>
-        <v>2.6466767341524537</v>
+        <v>2.5363985368961015</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -5809,11 +5853,11 @@
       </c>
       <c r="S21" s="56">
         <f>S20/(S19*$G$9*$H$9)</f>
-        <v>2.2317905402908114</v>
+        <v>2.138799267778694</v>
       </c>
       <c r="T21" s="56">
         <f>T20/(T19*$G$9*$H$9)</f>
-        <v>2.2046562621161399</v>
+        <v>2.1127955845279676</v>
       </c>
       <c r="Z21" s="36"/>
       <c r="AA21" s="36"/>
@@ -6206,43 +6250,43 @@
       </c>
       <c r="C33" s="35">
         <f>C32/(C31*$G$9*$H$9)</f>
-        <v>2.7355552992734404</v>
+        <v>2.6215738284703805</v>
       </c>
       <c r="D33" s="35">
         <f t="shared" ref="D33:L33" si="0">D32/(D31*$G$9*$H$9)</f>
-        <v>2.6948803704656545</v>
+        <v>2.5825936883629188</v>
       </c>
       <c r="E33" s="35">
         <f t="shared" si="0"/>
-        <v>2.7041117450324608</v>
+        <v>2.5914404223227749</v>
       </c>
       <c r="F33" s="35">
         <f t="shared" si="0"/>
-        <v>2.6818561872909696</v>
+        <v>2.5701121794871793</v>
       </c>
       <c r="G33" s="35">
         <f t="shared" si="0"/>
-        <v>2.6828259145605626</v>
+        <v>2.5710415014538723</v>
       </c>
       <c r="H33" s="35">
         <f t="shared" si="0"/>
-        <v>2.675881256104419</v>
+        <v>2.5643862037667344</v>
       </c>
       <c r="I33" s="35">
         <f t="shared" si="0"/>
-        <v>2.6902495497813219</v>
+        <v>2.5781558185404334</v>
       </c>
       <c r="J33" s="35">
         <f t="shared" si="0"/>
-        <v>2.6795720835455934</v>
+        <v>2.5679232467311937</v>
       </c>
       <c r="K33" s="35">
         <f t="shared" si="0"/>
-        <v>2.6853556799819622</v>
+        <v>2.5734658599827136</v>
       </c>
       <c r="L33" s="35">
         <f t="shared" si="0"/>
-        <v>2.683179740328022</v>
+        <v>2.5713805844810209</v>
       </c>
       <c r="Q33" s="68" t="s">
         <v>98</v>
@@ -6252,43 +6296,43 @@
       </c>
       <c r="S33" s="59">
         <f>S32/(S31*$G$9*$H$9)</f>
-        <v>2.2974015950604576</v>
+        <v>2.2016765285996054</v>
       </c>
       <c r="T33" s="59">
         <f t="shared" ref="T33:AB33" si="1">T32/(T31*$G$9*$H$9)</f>
-        <v>2.2676598763555282</v>
+        <v>2.1731740481740482</v>
       </c>
       <c r="U33" s="59">
         <f t="shared" si="1"/>
-        <v>2.2536970624974817</v>
+        <v>2.1597930182267535</v>
       </c>
       <c r="V33" s="59">
         <f t="shared" si="1"/>
-        <v>2.2478970305057264</v>
+        <v>2.1542346542346547</v>
       </c>
       <c r="W33" s="59">
         <f t="shared" si="1"/>
-        <v>2.2328975372453632</v>
+        <v>2.1398601398601391</v>
       </c>
       <c r="X33" s="59">
         <f t="shared" si="1"/>
-        <v>2.2336923603613092</v>
+        <v>2.1406218453462547</v>
       </c>
       <c r="Y33" s="59">
         <f t="shared" si="1"/>
-        <v>2.2343886012736522</v>
+        <v>2.1412890762205832</v>
       </c>
       <c r="Z33" s="59">
         <f t="shared" si="1"/>
-        <v>2.2180360236934362</v>
+        <v>2.1256178560395429</v>
       </c>
       <c r="AA33" s="59">
         <f t="shared" si="1"/>
-        <v>2.2214673913043481</v>
+        <v>2.12890625</v>
       </c>
       <c r="AB33" s="59">
         <f t="shared" si="1"/>
-        <v>2.2253986316768204</v>
+        <v>2.1326736886902862</v>
       </c>
     </row>
     <row r="34" spans="1:28" x14ac:dyDescent="0.35">
@@ -6920,43 +6964,43 @@
       </c>
       <c r="C45" s="35">
         <f>C44/(C43*$G$9*$H$9)</f>
-        <v>2.6559546313799625</v>
+        <v>2.5452898550724639</v>
       </c>
       <c r="D45" s="35">
         <f t="shared" ref="D45:L45" si="4">D44/(D43*$G$9*$H$9)</f>
-        <v>2.6474116620619457</v>
+        <v>2.5371028428093645</v>
       </c>
       <c r="E45" s="35">
         <f t="shared" si="4"/>
-        <v>2.648732956007203</v>
+        <v>2.5383690828402363</v>
       </c>
       <c r="F45" s="35">
         <f t="shared" si="4"/>
-        <v>2.6409406541985989</v>
+        <v>2.5309014602736579</v>
       </c>
       <c r="G45" s="35">
         <f t="shared" si="4"/>
-        <v>2.6451291539173125</v>
+        <v>2.5349154391707582</v>
       </c>
       <c r="H45" s="35">
         <f t="shared" si="4"/>
-        <v>2.6420072219483273</v>
+        <v>2.5319235877004802</v>
       </c>
       <c r="I45" s="35">
         <f t="shared" si="4"/>
-        <v>2.6387959866220729</v>
+        <v>2.5288461538461537</v>
       </c>
       <c r="J45" s="35">
         <f t="shared" si="4"/>
-        <v>2.6442307692307692</v>
+        <v>2.5340544871794872</v>
       </c>
       <c r="K45" s="35">
         <f t="shared" si="4"/>
-        <v>2.6543878656554716</v>
+        <v>2.5437883712531599</v>
       </c>
       <c r="L45" s="35">
         <f t="shared" si="4"/>
-        <v>2.6558380038124807</v>
+        <v>2.5451780869869602</v>
       </c>
       <c r="Q45" s="68" t="s">
         <v>98</v>
@@ -6966,43 +7010,43 @@
       </c>
       <c r="S45" s="59">
         <f>S44/(S43*$G$9*$H$9)</f>
-        <v>2.2145548452648067</v>
+        <v>2.1222817267121061</v>
       </c>
       <c r="T45" s="59">
         <f t="shared" ref="T45:AB45" si="5">T44/(T43*$G$9*$H$9)</f>
-        <v>2.2075259239340514</v>
+        <v>2.1155456771034657</v>
       </c>
       <c r="U45" s="59">
         <f t="shared" si="5"/>
-        <v>2.1955447823018628</v>
+        <v>2.1040637497059516</v>
       </c>
       <c r="V45" s="59">
         <f t="shared" si="5"/>
-        <v>2.2055898516346701</v>
+        <v>2.1136902744832256</v>
       </c>
       <c r="W45" s="59">
         <f t="shared" si="5"/>
-        <v>2.2020179309181867</v>
+        <v>2.1102671837965956</v>
       </c>
       <c r="X45" s="59">
         <f t="shared" si="5"/>
-        <v>2.2014479321970155</v>
+        <v>2.10972093502214</v>
       </c>
       <c r="Y45" s="59">
         <f t="shared" si="5"/>
-        <v>2.2032573456861311</v>
+        <v>2.1114549562825422</v>
       </c>
       <c r="Z45" s="59">
         <f t="shared" si="5"/>
-        <v>2.200217954981023</v>
+        <v>2.1085422068568138</v>
       </c>
       <c r="AA45" s="59">
         <f t="shared" si="5"/>
-        <v>2.2025629038251759</v>
+        <v>2.1107894494991268</v>
       </c>
       <c r="AB45" s="59">
         <f t="shared" si="5"/>
-        <v>2.2149256646241731</v>
+        <v>2.1226370952648321</v>
       </c>
     </row>
     <row r="46" spans="1:28" x14ac:dyDescent="0.35">
@@ -7413,55 +7457,55 @@
     </row>
     <row r="54" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A54" s="9"/>
-      <c r="B54" s="86" t="s">
+      <c r="B54" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="C54" s="86"/>
-      <c r="D54" s="86"/>
-      <c r="E54" s="86"/>
-      <c r="F54" s="86"/>
-      <c r="G54" s="86"/>
+      <c r="C54" s="104"/>
+      <c r="D54" s="104"/>
+      <c r="E54" s="104"/>
+      <c r="F54" s="104"/>
+      <c r="G54" s="104"/>
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
       <c r="Q54" s="45"/>
-      <c r="R54" s="90" t="s">
+      <c r="R54" s="108" t="s">
         <v>24</v>
       </c>
-      <c r="S54" s="90"/>
-      <c r="T54" s="90"/>
-      <c r="U54" s="90"/>
-      <c r="V54" s="90"/>
-      <c r="W54" s="90"/>
+      <c r="S54" s="108"/>
+      <c r="T54" s="108"/>
+      <c r="U54" s="108"/>
+      <c r="V54" s="108"/>
+      <c r="W54" s="108"/>
     </row>
     <row r="55" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A55" s="9"/>
-      <c r="B55" s="93" t="s">
+      <c r="B55" s="111" t="s">
         <v>55</v>
       </c>
-      <c r="C55" s="94"/>
-      <c r="D55" s="95"/>
-      <c r="E55" s="96" t="s">
+      <c r="C55" s="112"/>
+      <c r="D55" s="113"/>
+      <c r="E55" s="114" t="s">
         <v>1</v>
       </c>
-      <c r="F55" s="94"/>
-      <c r="G55" s="95"/>
+      <c r="F55" s="112"/>
+      <c r="G55" s="113"/>
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
       <c r="L55" s="1"/>
       <c r="Q55" s="45"/>
-      <c r="R55" s="98" t="s">
+      <c r="R55" s="116" t="s">
         <v>55</v>
       </c>
-      <c r="S55" s="99"/>
-      <c r="T55" s="100"/>
-      <c r="U55" s="101" t="s">
+      <c r="S55" s="117"/>
+      <c r="T55" s="118"/>
+      <c r="U55" s="119" t="s">
         <v>1</v>
       </c>
-      <c r="V55" s="99"/>
-      <c r="W55" s="100"/>
+      <c r="V55" s="117"/>
+      <c r="W55" s="118"/>
       <c r="Y55" s="36"/>
       <c r="Z55" s="36"/>
       <c r="AA55" s="36"/>
@@ -7545,7 +7589,7 @@
       </c>
       <c r="G57" s="34">
         <f>F57/(E57*$G$9*$H$9)</f>
-        <v>2.7411406349398648</v>
+        <v>2.6269264418173703</v>
       </c>
       <c r="H57" s="63"/>
       <c r="I57" s="1"/>
@@ -7577,7 +7621,7 @@
       </c>
       <c r="W57" s="56">
         <f>V57/(U57*$G$9*$H$9)</f>
-        <v>2.2026722461400658</v>
+        <v>2.1108942358842295</v>
       </c>
       <c r="X57" s="42"/>
       <c r="AC57" s="42"/>
@@ -7605,7 +7649,7 @@
       </c>
       <c r="G58" s="34">
         <f t="shared" ref="G58:G92" si="9">F58/(E58*$G$9*$H$9)</f>
-        <v>2.6916380808778997</v>
+        <v>2.5794864941746543</v>
       </c>
       <c r="H58" s="63"/>
       <c r="I58" s="1"/>
@@ -7637,7 +7681,7 @@
       </c>
       <c r="W58" s="56">
         <f t="shared" ref="W58:W92" si="11">V58/(U58*$G$9*$H$9)</f>
-        <v>2.272967464802528</v>
+        <v>2.1782604871024227</v>
       </c>
       <c r="X58" s="42"/>
       <c r="AC58" s="42"/>
@@ -7665,7 +7709,7 @@
       </c>
       <c r="G59" s="34">
         <f t="shared" si="9"/>
-        <v>2.7452667036713385</v>
+        <v>2.6308805910183657</v>
       </c>
       <c r="H59" s="63"/>
       <c r="I59" s="1"/>
@@ -7697,7 +7741,7 @@
       </c>
       <c r="W59" s="56">
         <f t="shared" si="11"/>
-        <v>2.3504286598091855</v>
+        <v>2.2524941323171359</v>
       </c>
       <c r="X59" s="42"/>
       <c r="AC59" s="42"/>
@@ -7725,7 +7769,7 @@
       </c>
       <c r="G60" s="34">
         <f t="shared" si="9"/>
-        <v>2.7009448564244285</v>
+        <v>2.5884054874067441</v>
       </c>
       <c r="H60" s="63"/>
       <c r="I60" s="1"/>
@@ -7757,7 +7801,7 @@
       </c>
       <c r="W60" s="56">
         <f t="shared" si="11"/>
-        <v>2.2444010068898681</v>
+        <v>2.1508842982694567</v>
       </c>
       <c r="X60" s="42"/>
       <c r="AC60" s="42"/>
@@ -7785,7 +7829,7 @@
       </c>
       <c r="G61" s="34">
         <f t="shared" si="9"/>
-        <v>2.8232628585361623</v>
+        <v>2.7056269060971552</v>
       </c>
       <c r="H61" s="63"/>
       <c r="I61" s="1"/>
@@ -7817,7 +7861,7 @@
       </c>
       <c r="W61" s="56">
         <f t="shared" si="11"/>
-        <v>2.3802277534215115</v>
+        <v>2.2810515970289487</v>
       </c>
       <c r="X61" s="42"/>
       <c r="AC61" s="42"/>
@@ -7845,7 +7889,7 @@
       </c>
       <c r="G62" s="34">
         <f t="shared" si="9"/>
-        <v>2.5975419713344228</v>
+        <v>2.4893110558621547</v>
       </c>
       <c r="H62" s="63"/>
       <c r="I62" s="1"/>
@@ -7876,7 +7920,7 @@
       </c>
       <c r="W62" s="56">
         <f t="shared" si="11"/>
-        <v>2.2547538726964067</v>
+        <v>2.16080579466739</v>
       </c>
       <c r="X62" s="42"/>
       <c r="AC62" s="42"/>
@@ -7904,7 +7948,7 @@
       </c>
       <c r="G63" s="34">
         <f t="shared" si="9"/>
-        <v>2.8011427265068889</v>
+        <v>2.6844284462357684</v>
       </c>
       <c r="H63" s="63"/>
       <c r="I63" s="1"/>
@@ -7936,7 +7980,7 @@
       </c>
       <c r="W63" s="56">
         <f t="shared" si="11"/>
-        <v>2.3245135425295209</v>
+        <v>2.2276588115907909</v>
       </c>
       <c r="X63" s="42"/>
       <c r="AC63" s="42"/>
@@ -7964,7 +8008,7 @@
       </c>
       <c r="G64" s="34">
         <f t="shared" si="9"/>
-        <v>2.7944018783981814</v>
+        <v>2.6779684667982573</v>
       </c>
       <c r="H64" s="63"/>
       <c r="I64" s="1"/>
@@ -7996,7 +8040,7 @@
       </c>
       <c r="W64" s="56">
         <f t="shared" si="11"/>
-        <v>2.1432096480160099</v>
+        <v>2.0539092460153427</v>
       </c>
       <c r="X64" s="42"/>
       <c r="AC64" s="42"/>
@@ -8024,7 +8068,7 @@
       </c>
       <c r="G65" s="34">
         <f t="shared" si="9"/>
-        <v>2.5583687110116657</v>
+        <v>2.4517700147195129</v>
       </c>
       <c r="H65" s="63"/>
       <c r="I65" s="1"/>
@@ -8056,7 +8100,7 @@
       </c>
       <c r="W65" s="56">
         <f t="shared" si="11"/>
-        <v>2.1820428169979915</v>
+        <v>2.0911243662897414</v>
       </c>
       <c r="X65" s="42"/>
       <c r="AC65" s="42"/>
@@ -8084,7 +8128,7 @@
       </c>
       <c r="G66" s="34">
         <f t="shared" si="9"/>
-        <v>2.5694059917759087</v>
+        <v>2.4623474087852459</v>
       </c>
       <c r="H66" s="63"/>
       <c r="I66" s="1"/>
@@ -8116,7 +8160,7 @@
       </c>
       <c r="W66" s="56">
         <f t="shared" si="11"/>
-        <v>2.0899530002308437</v>
+        <v>2.0028716252212257</v>
       </c>
       <c r="X66" s="42"/>
       <c r="AC66" s="42"/>
@@ -8144,7 +8188,7 @@
       </c>
       <c r="G67" s="34">
         <f t="shared" si="9"/>
-        <v>2.5778915112179099</v>
+        <v>2.4704793649171641</v>
       </c>
       <c r="H67" s="63"/>
       <c r="I67" s="1"/>
@@ -8176,7 +8220,7 @@
       </c>
       <c r="W67" s="56">
         <f t="shared" si="11"/>
-        <v>2.15594069727744</v>
+        <v>2.06610983489088</v>
       </c>
       <c r="X67" s="42"/>
       <c r="AC67" s="42"/>
@@ -8204,7 +8248,7 @@
       </c>
       <c r="G68" s="34">
         <f t="shared" si="9"/>
-        <v>2.5764127257105409</v>
+        <v>2.4690621954726018</v>
       </c>
       <c r="H68" s="63"/>
       <c r="I68" s="1"/>
@@ -8236,7 +8280,7 @@
       </c>
       <c r="W68" s="56">
         <f t="shared" si="11"/>
-        <v>2.1213038205545862</v>
+        <v>2.0329161613648119</v>
       </c>
       <c r="X68" s="42"/>
       <c r="AC68" s="42"/>
@@ -8264,7 +8308,7 @@
       </c>
       <c r="G69" s="34">
         <f t="shared" si="9"/>
-        <v>2.7087785320554234</v>
+        <v>2.5959127598864473</v>
       </c>
       <c r="H69" s="63"/>
       <c r="I69" s="1"/>
@@ -8296,7 +8340,7 @@
       </c>
       <c r="W69" s="56">
         <f t="shared" si="11"/>
-        <v>2.288148869208448</v>
+        <v>2.1928093329914291</v>
       </c>
       <c r="X69" s="42"/>
       <c r="AC69" s="42"/>
@@ -8324,7 +8368,7 @@
       </c>
       <c r="G70" s="34">
         <f t="shared" si="9"/>
-        <v>2.7659209648320178</v>
+        <v>2.6506742579640168</v>
       </c>
       <c r="H70" s="63"/>
       <c r="I70" s="1"/>
@@ -8356,7 +8400,7 @@
       </c>
       <c r="W70" s="56">
         <f t="shared" si="11"/>
-        <v>2.362776744645823</v>
+        <v>2.2643277136189139</v>
       </c>
       <c r="X70" s="42"/>
       <c r="AC70" s="42"/>
@@ -8384,7 +8428,7 @@
       </c>
       <c r="G71" s="34">
         <f t="shared" si="9"/>
-        <v>2.7521823009397215</v>
+        <v>2.6375080384005667</v>
       </c>
       <c r="H71" s="63"/>
       <c r="I71" s="1"/>
@@ -8416,7 +8460,7 @@
       </c>
       <c r="W71" s="56">
         <f t="shared" si="11"/>
-        <v>2.3799682914938254</v>
+        <v>2.2808029460149157</v>
       </c>
       <c r="X71" s="42"/>
       <c r="AC71" s="42"/>
@@ -8444,7 +8488,7 @@
       </c>
       <c r="G72" s="34">
         <f t="shared" si="9"/>
-        <v>2.6463058912565227</v>
+        <v>2.5360431457875006</v>
       </c>
       <c r="H72" s="63"/>
       <c r="I72" s="1"/>
@@ -8476,7 +8520,7 @@
       </c>
       <c r="W72" s="56">
         <f t="shared" si="11"/>
-        <v>2.2175381445857596</v>
+        <v>2.1251407218946863</v>
       </c>
       <c r="X72" s="42"/>
       <c r="AC72" s="42"/>
@@ -8504,7 +8548,7 @@
       </c>
       <c r="G73" s="34">
         <f t="shared" si="9"/>
-        <v>2.6684277246586761</v>
+        <v>2.5572432361312312</v>
       </c>
       <c r="H73" s="63"/>
       <c r="I73" s="1"/>
@@ -8536,7 +8580,7 @@
       </c>
       <c r="W73" s="56">
         <f t="shared" si="11"/>
-        <v>2.2028716444285847</v>
+        <v>2.1110853259107274</v>
       </c>
       <c r="X73" s="42"/>
       <c r="AC73" s="42"/>
@@ -8564,7 +8608,7 @@
       </c>
       <c r="G74" s="34">
         <f t="shared" si="9"/>
-        <v>3.0101851968574818</v>
+        <v>2.8847608136550869</v>
       </c>
       <c r="H74" s="63"/>
       <c r="I74" s="1"/>
@@ -8596,7 +8640,7 @@
       </c>
       <c r="W74" s="56">
         <f t="shared" si="11"/>
-        <v>2.4679114920657295</v>
+        <v>2.3650818465629908</v>
       </c>
       <c r="X74" s="42"/>
       <c r="AC74" s="42"/>
@@ -8624,7 +8668,7 @@
       </c>
       <c r="G75" s="34">
         <f t="shared" si="9"/>
-        <v>3.6802299214951799</v>
+        <v>3.526887008099548</v>
       </c>
       <c r="H75" s="63"/>
       <c r="I75" s="1"/>
@@ -8656,7 +8700,7 @@
       </c>
       <c r="W75" s="56">
         <f t="shared" si="11"/>
-        <v>3.3761061641485455</v>
+        <v>3.2354350739756894</v>
       </c>
       <c r="X75" s="42"/>
       <c r="AC75" s="42"/>
@@ -8684,7 +8728,7 @@
       </c>
       <c r="G76" s="34">
         <f t="shared" si="9"/>
-        <v>2.6701073905843082</v>
+        <v>2.5588529159766287</v>
       </c>
       <c r="H76" s="63"/>
       <c r="I76" s="1"/>
@@ -8716,7 +8760,7 @@
       </c>
       <c r="W76" s="56">
         <f t="shared" si="11"/>
-        <v>2.2147799362006082</v>
+        <v>2.1224974388589164</v>
       </c>
       <c r="X76" s="42"/>
       <c r="AC76" s="42"/>
@@ -8744,7 +8788,7 @@
       </c>
       <c r="G77" s="34">
         <f t="shared" si="9"/>
-        <v>2.6472710882726131</v>
+        <v>2.5369681262612547</v>
       </c>
       <c r="H77" s="63"/>
       <c r="I77" s="1"/>
@@ -8776,7 +8820,7 @@
       </c>
       <c r="W77" s="56">
         <f t="shared" si="11"/>
-        <v>2.1701149175043453</v>
+        <v>2.0796934626083305</v>
       </c>
       <c r="X77" s="42"/>
       <c r="AC77" s="42"/>
@@ -8804,7 +8848,7 @@
       </c>
       <c r="G78" s="34">
         <f t="shared" si="9"/>
-        <v>2.9205886768015059</v>
+        <v>2.7988974819347763</v>
       </c>
       <c r="H78" s="63"/>
       <c r="I78" s="1"/>
@@ -8836,7 +8880,7 @@
       </c>
       <c r="W78" s="56">
         <f t="shared" si="11"/>
-        <v>2.6583406374209573</v>
+        <v>2.5475764441950846</v>
       </c>
       <c r="X78" s="42"/>
       <c r="AC78" s="42"/>
@@ -8864,7 +8908,7 @@
       </c>
       <c r="G79" s="34">
         <f t="shared" si="9"/>
-        <v>2.8212121212121208</v>
+        <v>2.7036616161616163</v>
       </c>
       <c r="H79" s="63"/>
       <c r="I79" s="1"/>
@@ -8896,7 +8940,7 @@
       </c>
       <c r="W79" s="56">
         <f t="shared" si="11"/>
-        <v>2.5132128525136164</v>
+        <v>2.4084956503255492</v>
       </c>
       <c r="X79" s="42"/>
       <c r="AC79" s="42"/>
@@ -8924,7 +8968,7 @@
       </c>
       <c r="G80" s="34">
         <f t="shared" si="9"/>
-        <v>2.3183215183281254</v>
+        <v>2.2217247883977871</v>
       </c>
       <c r="H80" s="63"/>
       <c r="I80" s="1"/>
@@ -8956,7 +9000,7 @@
       </c>
       <c r="W80" s="56">
         <f t="shared" si="11"/>
-        <v>2.2647731322719187</v>
+        <v>2.1704075850939226</v>
       </c>
       <c r="X80" s="42"/>
       <c r="AC80" s="42"/>
@@ -8984,7 +9028,7 @@
       </c>
       <c r="G81" s="34">
         <f t="shared" si="9"/>
-        <v>2.88225238825168</v>
+        <v>2.7621585387411938</v>
       </c>
       <c r="H81" s="63"/>
       <c r="I81" s="1"/>
@@ -9016,7 +9060,7 @@
       </c>
       <c r="W81" s="56">
         <f t="shared" si="11"/>
-        <v>2.6887297965312658</v>
+        <v>2.5766993883424631</v>
       </c>
       <c r="X81" s="42"/>
       <c r="AC81" s="42"/>
@@ -9044,7 +9088,7 @@
       </c>
       <c r="G82" s="34">
         <f t="shared" si="9"/>
-        <v>2.6511655083047319</v>
+        <v>2.5407002787920354</v>
       </c>
       <c r="H82" s="63"/>
       <c r="I82" s="1"/>
@@ -9076,7 +9120,7 @@
       </c>
       <c r="W82" s="56">
         <f t="shared" si="11"/>
-        <v>2.2123703997514861</v>
+        <v>2.1201882997618404</v>
       </c>
       <c r="X82" s="42"/>
       <c r="AC82" s="42"/>
@@ -9104,7 +9148,7 @@
       </c>
       <c r="G83" s="34">
         <f t="shared" si="9"/>
-        <v>2.6398719394359249</v>
+        <v>2.5298772752927619</v>
       </c>
       <c r="H83" s="63"/>
       <c r="I83" s="1"/>
@@ -9136,7 +9180,7 @@
       </c>
       <c r="W83" s="56">
         <f t="shared" si="11"/>
-        <v>2.2753962114523247</v>
+        <v>2.1805880359751448</v>
       </c>
       <c r="X83" s="42"/>
       <c r="AC83" s="42"/>
@@ -9164,7 +9208,7 @@
       </c>
       <c r="G84" s="34">
         <f t="shared" si="9"/>
-        <v>2.6630652129931498</v>
+        <v>2.552104162451768</v>
       </c>
       <c r="H84" s="63"/>
       <c r="I84" s="1"/>
@@ -9196,7 +9240,7 @@
       </c>
       <c r="W84" s="56">
         <f t="shared" si="11"/>
-        <v>2.1641416901528054</v>
+        <v>2.0739691197297718</v>
       </c>
       <c r="X84" s="42"/>
       <c r="AC84" s="42"/>
@@ -9224,7 +9268,7 @@
       </c>
       <c r="G85" s="34">
         <f t="shared" si="9"/>
-        <v>2.5998175754762833</v>
+        <v>2.4914918431647712</v>
       </c>
       <c r="H85" s="63"/>
       <c r="I85" s="1"/>
@@ -9256,7 +9300,7 @@
       </c>
       <c r="W85" s="56">
         <f t="shared" si="11"/>
-        <v>2.1488733475587329</v>
+        <v>2.059336958077119</v>
       </c>
       <c r="X85" s="42"/>
       <c r="AC85" s="42"/>
@@ -9284,7 +9328,7 @@
       </c>
       <c r="G86" s="34">
         <f t="shared" si="9"/>
-        <v>3.136314147306587</v>
+        <v>3.0056343911688126</v>
       </c>
       <c r="H86" s="63"/>
       <c r="I86" s="1"/>
@@ -9316,7 +9360,7 @@
       </c>
       <c r="W86" s="56">
         <f t="shared" si="11"/>
-        <v>2.8831605660424118</v>
+        <v>2.7630288757906447</v>
       </c>
       <c r="X86" s="42"/>
       <c r="AC86" s="42"/>
@@ -9344,7 +9388,7 @@
       </c>
       <c r="G87" s="34">
         <f t="shared" si="9"/>
-        <v>2.680234846228593</v>
+        <v>2.5685583943024013</v>
       </c>
       <c r="H87" s="63"/>
       <c r="I87" s="1"/>
@@ -9376,7 +9420,7 @@
       </c>
       <c r="W87" s="56">
         <f t="shared" si="11"/>
-        <v>2.2433417390680379</v>
+        <v>2.1498691666068694</v>
       </c>
       <c r="X87" s="42"/>
       <c r="AC87" s="42"/>
@@ -9404,7 +9448,7 @@
       </c>
       <c r="G88" s="34">
         <f t="shared" si="9"/>
-        <v>2.8023820209960619</v>
+        <v>2.6856161034545596</v>
       </c>
       <c r="H88" s="63"/>
       <c r="I88" s="1"/>
@@ -9436,7 +9480,7 @@
       </c>
       <c r="W88" s="56">
         <f t="shared" si="11"/>
-        <v>2.2497111758671138</v>
+        <v>2.1559732102059841</v>
       </c>
       <c r="X88" s="42"/>
       <c r="AC88" s="42"/>
@@ -9464,7 +9508,7 @@
       </c>
       <c r="G89" s="34">
         <f t="shared" si="9"/>
-        <v>2.9696194824011743</v>
+        <v>2.8458853373011257</v>
       </c>
       <c r="H89" s="63"/>
       <c r="I89" s="1"/>
@@ -9496,7 +9540,7 @@
       </c>
       <c r="W89" s="56">
         <f t="shared" si="11"/>
-        <v>2.5343945614289307</v>
+        <v>2.4287947880360585</v>
       </c>
       <c r="X89" s="42"/>
       <c r="AC89" s="42"/>
@@ -9524,7 +9568,7 @@
       </c>
       <c r="G90" s="34">
         <f t="shared" si="9"/>
-        <v>2.6889594160627008</v>
+        <v>2.5769194403934219</v>
       </c>
       <c r="H90" s="63"/>
       <c r="I90" s="1"/>
@@ -9556,7 +9600,7 @@
       </c>
       <c r="W90" s="56">
         <f t="shared" si="11"/>
-        <v>2.2118685428824345</v>
+        <v>2.1197073535956665</v>
       </c>
       <c r="X90" s="42"/>
       <c r="AC90" s="42"/>
@@ -9584,7 +9628,7 @@
       </c>
       <c r="G91" s="34">
         <f t="shared" si="9"/>
-        <v>2.6565619620973817</v>
+        <v>2.5458718803433236</v>
       </c>
       <c r="H91" s="63"/>
       <c r="I91" s="1"/>
@@ -9616,7 +9660,7 @@
       </c>
       <c r="W91" s="56">
         <f t="shared" si="11"/>
-        <v>2.1803837625409201</v>
+        <v>2.0895344391017154</v>
       </c>
       <c r="X91" s="42"/>
       <c r="AC91" s="42"/>
@@ -9644,7 +9688,7 @@
       </c>
       <c r="G92" s="34">
         <f t="shared" si="9"/>
-        <v>2.6522282055653443</v>
+        <v>2.5417186970001215</v>
       </c>
       <c r="H92" s="63"/>
       <c r="I92" s="1"/>
@@ -9676,7 +9720,7 @@
       </c>
       <c r="W92" s="56">
         <f t="shared" si="11"/>
-        <v>2.1971208025919067</v>
+        <v>2.105574102483911</v>
       </c>
       <c r="X92" s="42"/>
       <c r="AC92" s="42"/>
@@ -9784,14 +9828,14 @@
     </row>
     <row r="96" spans="1:30" s="36" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A96" s="9"/>
-      <c r="B96" s="86" t="s">
+      <c r="B96" s="104" t="s">
         <v>25</v>
       </c>
-      <c r="C96" s="86"/>
-      <c r="D96" s="86"/>
-      <c r="E96" s="86"/>
-      <c r="F96" s="86"/>
-      <c r="G96" s="86"/>
+      <c r="C96" s="104"/>
+      <c r="D96" s="104"/>
+      <c r="E96" s="104"/>
+      <c r="F96" s="104"/>
+      <c r="G96" s="104"/>
       <c r="H96" s="8"/>
       <c r="I96" s="8"/>
       <c r="J96" s="8"/>
@@ -9802,30 +9846,30 @@
       <c r="O96" s="54"/>
       <c r="P96" s="42"/>
       <c r="Q96" s="45"/>
-      <c r="R96" s="90" t="s">
+      <c r="R96" s="108" t="s">
         <v>25</v>
       </c>
-      <c r="S96" s="90"/>
-      <c r="T96" s="90"/>
-      <c r="U96" s="90"/>
-      <c r="V96" s="90"/>
-      <c r="W96" s="90"/>
+      <c r="S96" s="108"/>
+      <c r="T96" s="108"/>
+      <c r="U96" s="108"/>
+      <c r="V96" s="108"/>
+      <c r="W96" s="108"/>
       <c r="X96" s="42"/>
       <c r="AC96" s="42"/>
       <c r="AD96" s="55"/>
     </row>
     <row r="97" spans="1:30" s="36" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" s="9"/>
-      <c r="B97" s="93" t="s">
+      <c r="B97" s="111" t="s">
         <v>55</v>
       </c>
-      <c r="C97" s="94"/>
-      <c r="D97" s="95"/>
-      <c r="E97" s="96" t="s">
+      <c r="C97" s="112"/>
+      <c r="D97" s="113"/>
+      <c r="E97" s="114" t="s">
         <v>1</v>
       </c>
-      <c r="F97" s="94"/>
-      <c r="G97" s="95"/>
+      <c r="F97" s="112"/>
+      <c r="G97" s="113"/>
       <c r="H97" s="8"/>
       <c r="I97" s="1"/>
       <c r="J97" s="1"/>
@@ -9836,16 +9880,16 @@
       <c r="O97" s="54"/>
       <c r="P97" s="42"/>
       <c r="Q97" s="45"/>
-      <c r="R97" s="98" t="s">
+      <c r="R97" s="116" t="s">
         <v>55</v>
       </c>
-      <c r="S97" s="99"/>
-      <c r="T97" s="100"/>
-      <c r="U97" s="101" t="s">
+      <c r="S97" s="117"/>
+      <c r="T97" s="118"/>
+      <c r="U97" s="119" t="s">
         <v>1</v>
       </c>
-      <c r="V97" s="99"/>
-      <c r="W97" s="100"/>
+      <c r="V97" s="117"/>
+      <c r="W97" s="118"/>
       <c r="X97" s="42"/>
       <c r="AC97" s="42"/>
       <c r="AD97" s="55"/>
@@ -9928,7 +9972,7 @@
       </c>
       <c r="G99" s="34">
         <f t="shared" ref="G99:G134" si="13">F99/(E99*$G$9*$H$9)</f>
-        <v>2.7041028712622022</v>
+        <v>2.5914319182929435</v>
       </c>
       <c r="H99" s="8"/>
       <c r="I99" s="1"/>
@@ -9960,7 +10004,7 @@
       </c>
       <c r="W99" s="56">
         <f t="shared" ref="W99:W134" si="15">V99/(U99*$G$9*$H$9)</f>
-        <v>2.2877845533949661</v>
+        <v>2.1924601970035096</v>
       </c>
       <c r="X99" s="42"/>
       <c r="AC99" s="42"/>
@@ -9988,7 +10032,7 @@
       </c>
       <c r="G100" s="34">
         <f t="shared" si="13"/>
-        <v>2.6853574282677508</v>
+        <v>2.5734675354232608</v>
       </c>
       <c r="H100" s="8"/>
       <c r="I100" s="1"/>
@@ -10020,7 +10064,7 @@
       </c>
       <c r="W100" s="56">
         <f t="shared" si="15"/>
-        <v>2.266132617531416</v>
+        <v>2.171710425134274</v>
       </c>
       <c r="X100" s="42"/>
       <c r="AC100" s="42"/>
@@ -10048,7 +10092,7 @@
       </c>
       <c r="G101" s="34">
         <f t="shared" si="13"/>
-        <v>2.7042288175019276</v>
+        <v>2.591552616772681</v>
       </c>
       <c r="H101" s="8"/>
       <c r="I101" s="1"/>
@@ -10080,7 +10124,7 @@
       </c>
       <c r="W101" s="56">
         <f t="shared" si="15"/>
-        <v>2.4127358956781211</v>
+        <v>2.3122052333581995</v>
       </c>
       <c r="X101" s="42"/>
       <c r="AC101" s="42"/>
@@ -10108,7 +10152,7 @@
       </c>
       <c r="G102" s="34">
         <f t="shared" si="13"/>
-        <v>2.6930066144292009</v>
+        <v>2.5807980054946507</v>
       </c>
       <c r="H102" s="8"/>
       <c r="I102" s="1"/>
@@ -10140,7 +10184,7 @@
       </c>
       <c r="W102" s="56">
         <f t="shared" si="15"/>
-        <v>2.275232993002017</v>
+        <v>2.1804316182935994</v>
       </c>
       <c r="X102" s="42"/>
       <c r="AC102" s="42"/>
@@ -10168,7 +10212,7 @@
       </c>
       <c r="G103" s="34">
         <f t="shared" si="13"/>
-        <v>2.831029855639561</v>
+        <v>2.7130702783212457</v>
       </c>
       <c r="H103" s="8"/>
       <c r="I103" s="1"/>
@@ -10200,7 +10244,7 @@
       </c>
       <c r="W103" s="56">
         <f t="shared" si="15"/>
-        <v>2.3939452332888767</v>
+        <v>2.2941975152351737</v>
       </c>
       <c r="X103" s="42"/>
       <c r="AC103" s="42"/>
@@ -10227,7 +10271,7 @@
       </c>
       <c r="G104" s="34">
         <f t="shared" si="13"/>
-        <v>2.6284890735340376</v>
+        <v>2.5189686954701189</v>
       </c>
       <c r="H104" s="8"/>
       <c r="I104" s="1"/>
@@ -10259,7 +10303,7 @@
       </c>
       <c r="W104" s="56">
         <f t="shared" si="15"/>
-        <v>2.3073311442785132</v>
+        <v>2.2111923466002419</v>
       </c>
       <c r="X104" s="42"/>
       <c r="AC104" s="42"/>
@@ -10287,7 +10331,7 @@
       </c>
       <c r="G105" s="34">
         <f t="shared" si="13"/>
-        <v>2.7928090901515166</v>
+        <v>2.6764420447285371</v>
       </c>
       <c r="H105" s="8"/>
       <c r="I105" s="1"/>
@@ -10319,7 +10363,7 @@
       </c>
       <c r="W105" s="56">
         <f t="shared" si="15"/>
-        <v>2.2906819045775912</v>
+        <v>2.1952368252201913</v>
       </c>
       <c r="X105" s="42"/>
       <c r="AC105" s="42"/>
@@ -10347,7 +10391,7 @@
       </c>
       <c r="G106" s="34">
         <f t="shared" si="13"/>
-        <v>2.7077588090927867</v>
+        <v>2.5949355253805875</v>
       </c>
       <c r="H106" s="8"/>
       <c r="I106" s="1"/>
@@ -10379,7 +10423,7 @@
       </c>
       <c r="W106" s="56">
         <f t="shared" si="15"/>
-        <v>2.1691757580211961</v>
+        <v>2.0787934347703128</v>
       </c>
       <c r="X106" s="42"/>
       <c r="AC106" s="42"/>
@@ -10407,7 +10451,7 @@
       </c>
       <c r="G107" s="34">
         <f t="shared" si="13"/>
-        <v>2.5584919633127403</v>
+        <v>2.4518881315080425</v>
       </c>
       <c r="H107" s="8"/>
       <c r="I107" s="1"/>
@@ -10439,7 +10483,7 @@
       </c>
       <c r="W107" s="56">
         <f t="shared" si="15"/>
-        <v>2.164389018286188</v>
+        <v>2.0742061425242637</v>
       </c>
       <c r="X107" s="42"/>
       <c r="AC107" s="42"/>
@@ -10467,7 +10511,7 @@
       </c>
       <c r="G108" s="34">
         <f t="shared" si="13"/>
-        <v>2.5925580177177032</v>
+        <v>2.4845347669794653</v>
       </c>
       <c r="H108" s="8"/>
       <c r="I108" s="1"/>
@@ -10499,7 +10543,7 @@
       </c>
       <c r="W108" s="56">
         <f t="shared" si="15"/>
-        <v>2.0806898715803905</v>
+        <v>1.993994460264541</v>
       </c>
       <c r="X108" s="42"/>
       <c r="AC108" s="42"/>
@@ -10527,7 +10571,7 @@
       </c>
       <c r="G109" s="34">
         <f t="shared" si="13"/>
-        <v>2.5675820540743488</v>
+        <v>2.4605994684879176</v>
       </c>
       <c r="H109" s="8"/>
       <c r="I109" s="1"/>
@@ -10559,7 +10603,7 @@
       </c>
       <c r="W109" s="56">
         <f t="shared" si="15"/>
-        <v>2.2133740952223637</v>
+        <v>2.1211501745880983</v>
       </c>
       <c r="X109" s="42"/>
       <c r="AC109" s="42"/>
@@ -10587,7 +10631,7 @@
       </c>
       <c r="G110" s="34">
         <f t="shared" si="13"/>
-        <v>2.6007451830232275</v>
+        <v>2.4923808003972598</v>
       </c>
       <c r="H110" s="8"/>
       <c r="I110" s="1"/>
@@ -10619,7 +10663,7 @@
       </c>
       <c r="W110" s="56">
         <f t="shared" si="15"/>
-        <v>2.115070791398864</v>
+        <v>2.0269428417572444</v>
       </c>
       <c r="X110" s="42"/>
       <c r="AC110" s="42"/>
@@ -10647,7 +10691,7 @@
       </c>
       <c r="G111" s="34">
         <f t="shared" si="13"/>
-        <v>2.7394475388559885</v>
+        <v>2.6253038914036555</v>
       </c>
       <c r="H111" s="8"/>
       <c r="I111" s="1"/>
@@ -10679,7 +10723,7 @@
       </c>
       <c r="W111" s="56">
         <f t="shared" si="15"/>
-        <v>2.3748754424995546</v>
+        <v>2.2759222990620729</v>
       </c>
       <c r="X111" s="42"/>
       <c r="AC111" s="42"/>
@@ -10707,7 +10751,7 @@
       </c>
       <c r="G112" s="34">
         <f t="shared" si="13"/>
-        <v>2.7363215997602062</v>
+        <v>2.6223081997701976</v>
       </c>
       <c r="H112" s="8"/>
       <c r="I112" s="1"/>
@@ -10739,7 +10783,7 @@
       </c>
       <c r="W112" s="56">
         <f t="shared" si="15"/>
-        <v>2.3714382492037909</v>
+        <v>2.2726283221536328</v>
       </c>
       <c r="X112" s="42"/>
       <c r="AC112" s="42"/>
@@ -10767,7 +10811,7 @@
       </c>
       <c r="G113" s="34">
         <f t="shared" si="13"/>
-        <v>2.7578979232321692</v>
+        <v>2.6429855097641619</v>
       </c>
       <c r="H113" s="8"/>
       <c r="I113" s="1"/>
@@ -10799,7 +10843,7 @@
       </c>
       <c r="W113" s="56">
         <f t="shared" si="15"/>
-        <v>2.3248914568936114</v>
+        <v>2.2280209795230439</v>
       </c>
       <c r="X113" s="42"/>
       <c r="AC113" s="42"/>
@@ -10827,7 +10871,7 @@
       </c>
       <c r="G114" s="34">
         <f t="shared" si="13"/>
-        <v>2.6422797413837538</v>
+        <v>2.5321847521594303</v>
       </c>
       <c r="H114" s="8"/>
       <c r="I114" s="1"/>
@@ -10859,7 +10903,7 @@
       </c>
       <c r="W114" s="56">
         <f t="shared" si="15"/>
-        <v>2.1789499402182013</v>
+        <v>2.0881603593757769</v>
       </c>
       <c r="X114" s="42"/>
       <c r="AC114" s="42"/>
@@ -10887,7 +10931,7 @@
       </c>
       <c r="G115" s="34">
         <f t="shared" si="13"/>
-        <v>2.6136390038151101</v>
+        <v>2.5047373786561473</v>
       </c>
       <c r="H115" s="8"/>
       <c r="I115" s="1"/>
@@ -10919,7 +10963,7 @@
       </c>
       <c r="W115" s="56">
         <f t="shared" si="15"/>
-        <v>2.1914351860672707</v>
+        <v>2.1001253866478011</v>
       </c>
       <c r="X115" s="42"/>
       <c r="AC115" s="42"/>
@@ -10947,7 +10991,7 @@
       </c>
       <c r="G116" s="34">
         <f t="shared" si="13"/>
-        <v>3.0212981371320571</v>
+        <v>2.8954107147515549</v>
       </c>
       <c r="H116" s="8"/>
       <c r="I116" s="1"/>
@@ -10979,7 +11023,7 @@
       </c>
       <c r="W116" s="56">
         <f t="shared" si="15"/>
-        <v>2.554354493420262</v>
+        <v>2.4479230561944183</v>
       </c>
       <c r="X116" s="42"/>
       <c r="AC116" s="42"/>
@@ -11007,7 +11051,7 @@
       </c>
       <c r="G117" s="34">
         <f t="shared" si="13"/>
-        <v>3.7147562161621419</v>
+        <v>3.5599747071553862</v>
       </c>
       <c r="H117" s="8"/>
       <c r="I117" s="1"/>
@@ -11039,7 +11083,7 @@
       </c>
       <c r="W117" s="56">
         <f t="shared" si="15"/>
-        <v>3.325539369054503</v>
+        <v>3.1869752286772322</v>
       </c>
       <c r="X117" s="42"/>
       <c r="AC117" s="42"/>
@@ -11067,7 +11111,7 @@
       </c>
       <c r="G118" s="34">
         <f t="shared" si="13"/>
-        <v>2.6473179755298224</v>
+        <v>2.5370130598827467</v>
       </c>
       <c r="H118" s="8"/>
       <c r="I118" s="1"/>
@@ -11099,7 +11143,7 @@
       </c>
       <c r="W118" s="56">
         <f t="shared" si="15"/>
-        <v>2.2305567817665324</v>
+        <v>2.1376169158595939</v>
       </c>
       <c r="X118" s="42"/>
       <c r="AC118" s="42"/>
@@ -11127,7 +11171,7 @@
       </c>
       <c r="G119" s="34">
         <f t="shared" si="13"/>
-        <v>2.5925489415543725</v>
+        <v>2.4845260689896072</v>
       </c>
       <c r="H119" s="8"/>
       <c r="I119" s="1"/>
@@ -11159,7 +11203,7 @@
       </c>
       <c r="W119" s="56">
         <f t="shared" si="15"/>
-        <v>2.1519594664688122</v>
+        <v>2.062294488699278</v>
       </c>
       <c r="X119" s="42"/>
       <c r="AC119" s="42"/>
@@ -11187,7 +11231,7 @@
       </c>
       <c r="G120" s="34">
         <f t="shared" si="13"/>
-        <v>2.8770051888989778</v>
+        <v>2.7571299726948535</v>
       </c>
       <c r="H120" s="8"/>
       <c r="I120" s="1"/>
@@ -11219,7 +11263,7 @@
       </c>
       <c r="W120" s="56">
         <f t="shared" si="15"/>
-        <v>2.6569183408624717</v>
+        <v>2.5462134099932023</v>
       </c>
       <c r="X120" s="42"/>
       <c r="AC120" s="42"/>
@@ -11247,7 +11291,7 @@
       </c>
       <c r="G121" s="34">
         <f t="shared" si="13"/>
-        <v>2.7775418374975258</v>
+        <v>2.6618109276017954</v>
       </c>
       <c r="H121" s="8"/>
       <c r="I121" s="1"/>
@@ -11279,7 +11323,7 @@
       </c>
       <c r="W121" s="56">
         <f t="shared" si="15"/>
-        <v>2.492431734699641</v>
+        <v>2.3885804124204886</v>
       </c>
       <c r="X121" s="42"/>
       <c r="AC121" s="42"/>
@@ -11307,7 +11351,7 @@
       </c>
       <c r="G122" s="34">
         <f t="shared" si="13"/>
-        <v>2.3720832447770572</v>
+        <v>2.2732464429113466</v>
       </c>
       <c r="H122" s="8"/>
       <c r="I122" s="1"/>
@@ -11338,7 +11382,7 @@
       </c>
       <c r="W122" s="56">
         <f t="shared" si="15"/>
-        <v>2.2682041543260008</v>
+        <v>2.1736956478957503</v>
       </c>
       <c r="X122" s="42"/>
       <c r="AC122" s="42"/>
@@ -11366,7 +11410,7 @@
       </c>
       <c r="G123" s="34">
         <f t="shared" si="13"/>
-        <v>2.8384229661083591</v>
+        <v>2.7201553425205107</v>
       </c>
       <c r="H123" s="8"/>
       <c r="I123" s="1"/>
@@ -11398,7 +11442,7 @@
       </c>
       <c r="W123" s="56">
         <f t="shared" si="15"/>
-        <v>2.6583190282798426</v>
+        <v>2.5475557354348495</v>
       </c>
       <c r="X123" s="42"/>
       <c r="AC123" s="42"/>
@@ -11426,7 +11470,7 @@
       </c>
       <c r="G124" s="34">
         <f t="shared" si="13"/>
-        <v>2.6818102262427619</v>
+        <v>2.5700681334826467</v>
       </c>
       <c r="H124" s="8"/>
       <c r="I124" s="1"/>
@@ -11458,7 +11502,7 @@
       </c>
       <c r="W124" s="56">
         <f t="shared" si="15"/>
-        <v>2.2061279764249995</v>
+        <v>2.1142059774072912</v>
       </c>
       <c r="X124" s="42"/>
       <c r="AC124" s="42"/>
@@ -11486,7 +11530,7 @@
       </c>
       <c r="G125" s="34">
         <f t="shared" si="13"/>
-        <v>2.6595385570602024</v>
+        <v>2.5487244505160276</v>
       </c>
       <c r="H125" s="8"/>
       <c r="I125" s="1"/>
@@ -11518,7 +11562,7 @@
       </c>
       <c r="W125" s="56">
         <f t="shared" si="15"/>
-        <v>2.3029181468624267</v>
+        <v>2.2069632240764916</v>
       </c>
       <c r="X125" s="42"/>
       <c r="AC125" s="42"/>
@@ -11546,7 +11590,7 @@
       </c>
       <c r="G126" s="34">
         <f t="shared" si="13"/>
-        <v>2.6628169987591459</v>
+        <v>2.5518662904775145</v>
       </c>
       <c r="H126" s="8"/>
       <c r="I126" s="1"/>
@@ -11578,7 +11622,7 @@
       </c>
       <c r="W126" s="56">
         <f t="shared" si="15"/>
-        <v>2.1772483308595438</v>
+        <v>2.0865296504070625</v>
       </c>
       <c r="X126" s="42"/>
       <c r="AC126" s="42"/>
@@ -11606,7 +11650,7 @@
       </c>
       <c r="G127" s="34">
         <f t="shared" si="13"/>
-        <v>2.5841296736654957</v>
+        <v>2.476457603929433</v>
       </c>
       <c r="H127" s="8"/>
       <c r="I127" s="1"/>
@@ -11638,7 +11682,7 @@
       </c>
       <c r="W127" s="56">
         <f t="shared" si="15"/>
-        <v>2.1508744849437056</v>
+        <v>2.0612547147377183</v>
       </c>
       <c r="X127" s="42"/>
       <c r="AC127" s="42"/>
@@ -11666,7 +11710,7 @@
       </c>
       <c r="G128" s="34">
         <f t="shared" si="13"/>
-        <v>3.1086798887610554</v>
+        <v>2.9791515600626783</v>
       </c>
       <c r="H128" s="8"/>
       <c r="I128" s="1"/>
@@ -11698,7 +11742,7 @@
       </c>
       <c r="W128" s="56">
         <f t="shared" si="15"/>
-        <v>3.0339138035650004</v>
+        <v>2.9075007284164585</v>
       </c>
       <c r="X128" s="42"/>
       <c r="AC128" s="42"/>
@@ -11726,7 +11770,7 @@
       </c>
       <c r="G129" s="34">
         <f t="shared" si="13"/>
-        <v>2.6774321288559553</v>
+        <v>2.5658724568202906</v>
       </c>
       <c r="H129" s="8"/>
       <c r="I129" s="1"/>
@@ -11758,7 +11802,7 @@
       </c>
       <c r="W129" s="56">
         <f t="shared" si="15"/>
-        <v>2.2660109536141406</v>
+        <v>2.1715938305468843</v>
       </c>
       <c r="X129" s="42"/>
       <c r="AC129" s="42"/>
@@ -11786,7 +11830,7 @@
       </c>
       <c r="G130" s="34">
         <f t="shared" si="13"/>
-        <v>2.7954781797440527</v>
+        <v>2.6789999222547167</v>
       </c>
       <c r="H130" s="8"/>
       <c r="I130" s="1"/>
@@ -11818,7 +11862,7 @@
       </c>
       <c r="W130" s="56">
         <f t="shared" si="15"/>
-        <v>2.2673437572688395</v>
+        <v>2.1728711007159713</v>
       </c>
       <c r="X130" s="42"/>
       <c r="AC130" s="42"/>
@@ -11846,7 +11890,7 @@
       </c>
       <c r="G131" s="34">
         <f t="shared" si="13"/>
-        <v>2.9585183529378614</v>
+        <v>2.8352467548987841</v>
       </c>
       <c r="H131" s="8"/>
       <c r="I131" s="1"/>
@@ -11878,7 +11922,7 @@
       </c>
       <c r="W131" s="56">
         <f t="shared" si="15"/>
-        <v>2.5305059120675342</v>
+        <v>2.4250681657313873</v>
       </c>
       <c r="X131" s="42"/>
       <c r="AC131" s="42"/>
@@ -11906,7 +11950,7 @@
       </c>
       <c r="G132" s="34">
         <f t="shared" si="13"/>
-        <v>2.6364030751945191</v>
+        <v>2.5265529470614139</v>
       </c>
       <c r="H132" s="8"/>
       <c r="I132" s="1"/>
@@ -11938,7 +11982,7 @@
       </c>
       <c r="W132" s="56">
         <f t="shared" si="15"/>
-        <v>2.1639102072542031</v>
+        <v>2.0737472819519449</v>
       </c>
       <c r="X132" s="42"/>
       <c r="AC132" s="42"/>
@@ -11966,7 +12010,7 @@
       </c>
       <c r="G133" s="34">
         <f t="shared" si="13"/>
-        <v>2.622396374245882</v>
+        <v>2.5131298586523036</v>
       </c>
       <c r="H133" s="8"/>
       <c r="I133" s="1"/>
@@ -11998,7 +12042,7 @@
       </c>
       <c r="W133" s="56">
         <f t="shared" si="15"/>
-        <v>2.1372597247630134</v>
+        <v>2.0482072362312209</v>
       </c>
       <c r="X133" s="42"/>
       <c r="AC133" s="42"/>
@@ -12026,7 +12070,7 @@
       </c>
       <c r="G134" s="34">
         <f t="shared" si="13"/>
-        <v>2.6390455072276024</v>
+        <v>2.5290852777597856</v>
       </c>
       <c r="H134" s="8"/>
       <c r="I134" s="1"/>
@@ -12058,7 +12102,7 @@
       </c>
       <c r="W134" s="56">
         <f t="shared" si="15"/>
-        <v>2.1660354915727793</v>
+        <v>2.0757840127572464</v>
       </c>
       <c r="X134" s="42"/>
       <c r="AC134" s="42"/>
@@ -12385,9 +12429,9 @@
       <c r="AD144" s="55"/>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B150" s="97"/>
-      <c r="C150" s="97"/>
-      <c r="D150" s="97"/>
+      <c r="B150" s="115"/>
+      <c r="C150" s="115"/>
+      <c r="D150" s="115"/>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A151" s="15"/>
@@ -12600,10 +12644,451 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:AD18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C5" zoomScale="92" zoomScaleNormal="65" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18:Z18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.26953125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="12.54296875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="14.26953125" style="8" customWidth="1"/>
+    <col min="4" max="13" width="8.7265625" style="8"/>
+    <col min="14" max="14" width="8.7265625" style="14"/>
+    <col min="15" max="15" width="8.7265625" style="36"/>
+    <col min="16" max="16" width="15" style="36" customWidth="1"/>
+    <col min="17" max="30" width="8.7265625" style="36"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" ht="29" thickBot="1" x14ac:dyDescent="0.7">
+      <c r="A1" s="101" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="102"/>
+      <c r="E1" s="102"/>
+      <c r="F1" s="102"/>
+      <c r="G1" s="102"/>
+      <c r="H1" s="102"/>
+      <c r="I1" s="102"/>
+      <c r="J1" s="102"/>
+      <c r="K1" s="102"/>
+      <c r="L1" s="102"/>
+      <c r="M1" s="102"/>
+      <c r="N1" s="105"/>
+      <c r="O1" s="99" t="s">
+        <v>50</v>
+      </c>
+      <c r="P1" s="100"/>
+      <c r="Q1" s="100"/>
+      <c r="R1" s="100"/>
+      <c r="S1" s="100"/>
+      <c r="T1" s="100"/>
+      <c r="U1" s="100"/>
+      <c r="V1" s="100"/>
+      <c r="W1" s="100"/>
+      <c r="X1" s="100"/>
+      <c r="Y1" s="100"/>
+      <c r="Z1" s="100"/>
+      <c r="AA1" s="100"/>
+      <c r="AB1" s="100"/>
+      <c r="AC1" s="100"/>
+      <c r="AD1" s="103"/>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A3" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="P3" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q3" s="42"/>
+      <c r="R3" s="42"/>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A4" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="P4" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q4" s="43" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A5" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" s="88">
+        <f>6.3*12/14.2</f>
+        <v>5.323943661971831</v>
+      </c>
+      <c r="P5" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q5" s="91">
+        <f>6.67*12/14.2</f>
+        <v>5.6366197183098592</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A6" s="15"/>
+      <c r="P6" s="47"/>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A7" s="15"/>
+      <c r="P7" s="47"/>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A8" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="89" t="s">
+        <v>15</v>
+      </c>
+      <c r="P8" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q8" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="R8" s="48" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A9" s="95" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9" s="90">
+        <f>5.03*12/14.2</f>
+        <v>4.2507042253521128</v>
+      </c>
+      <c r="C9" s="87">
+        <f>9.03*12/14.2</f>
+        <v>7.6309859154929569</v>
+      </c>
+      <c r="P9" s="92" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q9" s="93">
+        <f>5.6*12/14.2</f>
+        <v>4.7323943661971821</v>
+      </c>
+      <c r="R9" s="94">
+        <f>8.79*12/14.2</f>
+        <v>7.4281690140845065</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A10" s="15"/>
+      <c r="P10" s="47"/>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A11" s="15"/>
+      <c r="P11" s="47"/>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A12" s="15"/>
+      <c r="P12" s="47"/>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A13" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2</v>
+      </c>
+      <c r="D13" s="2">
+        <v>3</v>
+      </c>
+      <c r="E13" s="2">
+        <v>4</v>
+      </c>
+      <c r="F13" s="2">
+        <v>5</v>
+      </c>
+      <c r="G13" s="2">
+        <v>6</v>
+      </c>
+      <c r="H13" s="2">
+        <v>7</v>
+      </c>
+      <c r="I13" s="2">
+        <v>8</v>
+      </c>
+      <c r="J13" s="2">
+        <v>9</v>
+      </c>
+      <c r="K13" s="2">
+        <v>10</v>
+      </c>
+      <c r="P13" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q13" s="43">
+        <v>1</v>
+      </c>
+      <c r="R13" s="43">
+        <v>2</v>
+      </c>
+      <c r="S13" s="43">
+        <v>3</v>
+      </c>
+      <c r="T13" s="43">
+        <v>4</v>
+      </c>
+      <c r="U13" s="43">
+        <v>5</v>
+      </c>
+      <c r="V13" s="43">
+        <v>6</v>
+      </c>
+      <c r="W13" s="43">
+        <v>7</v>
+      </c>
+      <c r="X13" s="43">
+        <v>8</v>
+      </c>
+      <c r="Y13" s="43">
+        <v>9</v>
+      </c>
+      <c r="Z13" s="43">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A14" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="34">
+        <v>1.4704225352112676</v>
+      </c>
+      <c r="C14" s="34">
+        <v>2.4</v>
+      </c>
+      <c r="D14" s="34">
+        <v>2.9999999999999996</v>
+      </c>
+      <c r="E14" s="34">
+        <v>3.3464788732394366</v>
+      </c>
+      <c r="F14" s="34">
+        <v>3.9126760563380287</v>
+      </c>
+      <c r="G14" s="34">
+        <v>4.2929577464788737</v>
+      </c>
+      <c r="H14" s="34">
+        <v>4.7492957746478872</v>
+      </c>
+      <c r="I14" s="34">
+        <v>5.1464788732394364</v>
+      </c>
+      <c r="J14" s="34">
+        <v>5.6704225352112676</v>
+      </c>
+      <c r="K14" s="34">
+        <v>6.0591549295774643</v>
+      </c>
+      <c r="P14" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q14" s="56">
+        <v>1.8760563380281692</v>
+      </c>
+      <c r="R14" s="56">
+        <v>3.042253521126761</v>
+      </c>
+      <c r="S14" s="56">
+        <v>3.6676056338028169</v>
+      </c>
+      <c r="T14" s="56">
+        <v>4.1154929577464792</v>
+      </c>
+      <c r="U14" s="56">
+        <v>4.394366197183099</v>
+      </c>
+      <c r="V14" s="56">
+        <v>4.8338028169014091</v>
+      </c>
+      <c r="W14" s="56">
+        <v>5.2309859154929583</v>
+      </c>
+      <c r="X14" s="56">
+        <v>5.5943661971830991</v>
+      </c>
+      <c r="Y14" s="56">
+        <v>6.0422535211267618</v>
+      </c>
+      <c r="Z14" s="56">
+        <v>6.3464788732394375</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A15" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="34">
+        <v>6.7014084507042257</v>
+      </c>
+      <c r="C15" s="34">
+        <v>7.8507042253521124</v>
+      </c>
+      <c r="D15" s="34">
+        <v>8.2563380281690133</v>
+      </c>
+      <c r="E15" s="34">
+        <v>8.4845070422535205</v>
+      </c>
+      <c r="F15" s="34">
+        <v>8.4591549295774655</v>
+      </c>
+      <c r="G15" s="34">
+        <v>8.3915492957746487</v>
+      </c>
+      <c r="H15" s="34">
+        <v>8.214084507042255</v>
+      </c>
+      <c r="I15" s="34">
+        <v>7.9352112676056343</v>
+      </c>
+      <c r="J15" s="34">
+        <v>7.4450704225352116</v>
+      </c>
+      <c r="K15" s="34">
+        <v>5.8056338028169012</v>
+      </c>
+      <c r="P15" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q15" s="56">
+        <v>7.0056338028169014</v>
+      </c>
+      <c r="R15" s="56">
+        <v>8.2225352112676067</v>
+      </c>
+      <c r="S15" s="56">
+        <v>8.3661971830985919</v>
+      </c>
+      <c r="T15" s="56">
+        <v>8.1718309859154932</v>
+      </c>
+      <c r="U15" s="56">
+        <v>8.2056338028169034</v>
+      </c>
+      <c r="V15" s="56">
+        <v>8.1295774647887331</v>
+      </c>
+      <c r="W15" s="56">
+        <v>8.0281690140845079</v>
+      </c>
+      <c r="X15" s="56">
+        <v>7.6985915492957746</v>
+      </c>
+      <c r="Y15" s="56">
+        <v>7.2422535211267611</v>
+      </c>
+      <c r="Z15" s="56">
+        <v>5.1464788732394364</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="P16" s="47"/>
+    </row>
+    <row r="17" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="B17" s="63"/>
+      <c r="C17" s="63"/>
+      <c r="D17" s="63"/>
+      <c r="E17" s="63"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="63"/>
+      <c r="I17" s="63"/>
+      <c r="J17" s="63"/>
+      <c r="K17" s="63"/>
+      <c r="P17" s="47"/>
+    </row>
+    <row r="18" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="B18" s="63"/>
+      <c r="C18" s="63"/>
+      <c r="D18" s="63"/>
+      <c r="E18" s="63"/>
+      <c r="F18" s="63"/>
+      <c r="G18" s="63"/>
+      <c r="H18" s="63"/>
+      <c r="I18" s="63"/>
+      <c r="J18" s="63"/>
+      <c r="K18" s="63"/>
+      <c r="Q18" s="40">
+        <f>Q14/Q15</f>
+        <v>0.26779252110977081</v>
+      </c>
+      <c r="R18" s="40">
+        <f t="shared" ref="R18:Z18" si="0">R14/R15</f>
+        <v>0.36998972250770812</v>
+      </c>
+      <c r="S18" s="40">
+        <f t="shared" si="0"/>
+        <v>0.43838383838383838</v>
+      </c>
+      <c r="T18" s="40">
+        <f t="shared" si="0"/>
+        <v>0.50361944157187177</v>
+      </c>
+      <c r="U18" s="40">
+        <f t="shared" si="0"/>
+        <v>0.53553038105046336</v>
+      </c>
+      <c r="V18" s="40">
+        <f t="shared" si="0"/>
+        <v>0.59459459459459463</v>
+      </c>
+      <c r="W18" s="40">
+        <f t="shared" si="0"/>
+        <v>0.65157894736842104</v>
+      </c>
+      <c r="X18" s="40">
+        <f t="shared" si="0"/>
+        <v>0.72667398463227229</v>
+      </c>
+      <c r="Y18" s="40">
+        <f t="shared" si="0"/>
+        <v>0.83430571761960337</v>
+      </c>
+      <c r="Z18" s="40">
+        <f t="shared" si="0"/>
+        <v>1.233169129720854</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="O1:AD1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="C4:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -12619,136 +13104,136 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C4" s="103" t="s">
+      <c r="C4" s="79" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="103" t="s">
+      <c r="D4" s="79" t="s">
         <v>117</v>
       </c>
-      <c r="E4" s="103" t="s">
+      <c r="E4" s="79" t="s">
         <v>111</v>
       </c>
-      <c r="F4" s="103" t="s">
+      <c r="F4" s="79" t="s">
         <v>116</v>
       </c>
-      <c r="G4" s="103" t="s">
+      <c r="G4" s="79" t="s">
         <v>123</v>
       </c>
-      <c r="H4" s="103" t="s">
+      <c r="H4" s="79" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="5" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C5" s="104" t="s">
+      <c r="C5" s="80" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="104" t="s">
+      <c r="D5" s="80" t="s">
         <v>109</v>
       </c>
-      <c r="E5" s="104" t="s">
+      <c r="E5" s="80" t="s">
         <v>112</v>
       </c>
-      <c r="F5" s="105">
-        <f>'Average consumption'!C6</f>
+      <c r="F5" s="81">
+        <f>'Average consumption - PC 30 day'!C6</f>
         <v>1.4733149999999999</v>
       </c>
-      <c r="G5" s="105">
-        <f>'Average consumption'!S6</f>
+      <c r="G5" s="81">
+        <f>'Average consumption - PC 30 day'!S6</f>
         <v>1.5981240000000001</v>
       </c>
-      <c r="H5" s="104" t="s">
+      <c r="H5" s="80" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C6" s="104" t="s">
+      <c r="C6" s="80" t="s">
         <v>120</v>
       </c>
-      <c r="D6" s="104" t="s">
+      <c r="D6" s="80" t="s">
         <v>110</v>
       </c>
-      <c r="E6" s="104" t="s">
+      <c r="E6" s="80" t="s">
         <v>113</v>
       </c>
-      <c r="F6" s="106">
+      <c r="F6" s="82">
         <v>143.81</v>
       </c>
-      <c r="G6" s="106">
+      <c r="G6" s="82">
         <v>143.81</v>
       </c>
-      <c r="H6" s="107" t="s">
+      <c r="H6" s="83" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="7" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C7" s="104" t="s">
+      <c r="C7" s="80" t="s">
         <v>108</v>
       </c>
-      <c r="D7" s="108" t="s">
+      <c r="D7" s="84" t="s">
         <v>114</v>
       </c>
-      <c r="E7" s="104" t="s">
+      <c r="E7" s="80" t="s">
         <v>115</v>
       </c>
-      <c r="F7" s="109">
+      <c r="F7" s="85">
         <f>F6*F5*12*(10^7)/(10^9)</f>
         <v>25.425291617999996</v>
       </c>
-      <c r="G7" s="109">
+      <c r="G7" s="85">
         <f>G6*G5*12*(10^7)/(10^9)</f>
         <v>27.579145492799999</v>
       </c>
-      <c r="H7" s="104" t="s">
+      <c r="H7" s="80" t="s">
         <v>122</v>
       </c>
-      <c r="J7" s="102"/>
+      <c r="J7" s="78"/>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C8" s="104" t="s">
+      <c r="C8" s="80" t="s">
         <v>128</v>
       </c>
-      <c r="D8" s="108" t="s">
+      <c r="D8" s="84" t="s">
         <v>114</v>
       </c>
-      <c r="E8" s="104" t="s">
+      <c r="E8" s="80" t="s">
         <v>124</v>
       </c>
-      <c r="F8" s="104">
+      <c r="F8" s="80">
         <v>25.61</v>
       </c>
-      <c r="G8" s="104">
+      <c r="G8" s="80">
         <v>26.47</v>
       </c>
-      <c r="H8" s="110" t="s">
+      <c r="H8" s="86" t="s">
         <v>127</v>
       </c>
-      <c r="J8" s="102"/>
+      <c r="J8" s="78"/>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C9" s="104" t="s">
+      <c r="C9" s="80" t="s">
         <v>125</v>
       </c>
-      <c r="D9" s="108" t="s">
+      <c r="D9" s="84" t="s">
         <v>114</v>
       </c>
-      <c r="E9" s="104" t="s">
+      <c r="E9" s="80" t="s">
         <v>126</v>
       </c>
-      <c r="F9" s="109">
+      <c r="F9" s="85">
         <f>F8-F7</f>
         <v>0.18470838200000372</v>
       </c>
-      <c r="G9" s="109">
+      <c r="G9" s="85">
         <f>G8-G7</f>
         <v>-1.1091454927999997</v>
       </c>
-      <c r="H9" s="104" t="s">
+      <c r="H9" s="80" t="s">
         <v>122</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H6" r:id="rId1"/>
+    <hyperlink ref="H6" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>